<commit_message>
Mise a jour Images 3Level AFE
Mise a jour de la commande avec les paramètres à Viarouge pour le 3
LEVEL AFE
Ajout fichier avec temps de simulation
</commit_message>
<xml_diff>
--- a/Remise/Documentation_technique/Temps_simulations1u.xlsx
+++ b/Remise/Documentation_technique/Temps_simulations1u.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Simulations</t>
   </si>
@@ -27,36 +27,71 @@
     <t>PSIM</t>
   </si>
   <si>
-    <t>AFE3LEVEL+DCP/DCN</t>
-  </si>
-  <si>
-    <t>AFE+HACHEUR</t>
-  </si>
-  <si>
-    <t>AFE2LEVELRC</t>
-  </si>
-  <si>
-    <t>AFE2LEVELIDEAL</t>
-  </si>
-  <si>
-    <t>DCP/DCN</t>
-  </si>
-  <si>
-    <t>HACHEUR</t>
-  </si>
-  <si>
     <t>23min</t>
   </si>
   <si>
     <t>22min</t>
+  </si>
+  <si>
+    <t>9min</t>
+  </si>
+  <si>
+    <t>4min</t>
+  </si>
+  <si>
+    <t>5min</t>
+  </si>
+  <si>
+    <t>AFE 3 LEVEL+DCP/DCN 0.9sec</t>
+  </si>
+  <si>
+    <t>AFE 2 LEVEL + HACHEUR 0.9sec</t>
+  </si>
+  <si>
+    <t>AFE 3 LEVEL PWM 1sec</t>
+  </si>
+  <si>
+    <t>AFE 2 LEVEL HYSTERESIS 1sec</t>
+  </si>
+  <si>
+    <t>DCP/DCN 0.9sec</t>
+  </si>
+  <si>
+    <t>6min</t>
+  </si>
+  <si>
+    <t>AFE 2 LEVEL IDEAL 1sec</t>
+  </si>
+  <si>
+    <t>7min</t>
+  </si>
+  <si>
+    <t>8min</t>
+  </si>
+  <si>
+    <t>1min</t>
+  </si>
+  <si>
+    <t>3min</t>
+  </si>
+  <si>
+    <t>HACHEUR 4 QUADRANTS 0.9sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,12 +115,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,65 +452,123 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Temps de simulation sur AMD FX-8350
</commit_message>
<xml_diff>
--- a/Remise/Documentation_technique/Temps_simulations1u.xlsx
+++ b/Remise/Documentation_technique/Temps_simulations1u.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\DesignIV\Remise\Documentation_technique\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="18915" windowHeight="8250"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Simulations</t>
   </si>
@@ -76,6 +81,51 @@
   </si>
   <si>
     <t>HACHEUR 4 QUADRANTS 0.9sec</t>
+  </si>
+  <si>
+    <t>GAB</t>
+  </si>
+  <si>
+    <t>16s</t>
+  </si>
+  <si>
+    <t>1m 41s</t>
+  </si>
+  <si>
+    <t>2m 48s</t>
+  </si>
+  <si>
+    <t>2m 49s</t>
+  </si>
+  <si>
+    <t>2m 5s</t>
+  </si>
+  <si>
+    <t>1m 19s</t>
+  </si>
+  <si>
+    <t>2m 33s</t>
+  </si>
+  <si>
+    <t>AMD FX-8350 4 GHz (Run 1)</t>
+  </si>
+  <si>
+    <t>1m 28s</t>
+  </si>
+  <si>
+    <t>4m 11s</t>
+  </si>
+  <si>
+    <t>7m 23s</t>
+  </si>
+  <si>
+    <t>3m 08s</t>
+  </si>
+  <si>
+    <t>1m 20s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5m 54s </t>
   </si>
 </sst>
 </file>
@@ -107,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -130,22 +180,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -158,12 +226,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -205,7 +276,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,123 +520,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A7:B7"/>
+  <mergeCells count="10">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -578,7 +711,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -590,7 +723,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>